<commit_message>
added pre travel request page
</commit_message>
<xml_diff>
--- a/wp-admin/error.xlsx
+++ b/wp-admin/error.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Employee Code</t>
   </si>
@@ -50,102 +50,6 @@
   </si>
   <si>
     <t>Error Message</t>
-  </si>
-  <si>
-    <t>tfv222</t>
-  </si>
-  <si>
-    <t>LP</t>
-  </si>
-  <si>
-    <t>slakshmiprasanna34@gmail.com</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>tfv3</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
-    <t>tfv4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Employee Email already Exists</t>
-  </si>
-  <si>
-    <t>tfv223</t>
-  </si>
-  <si>
-    <t>Rajani</t>
-  </si>
-  <si>
-    <t>rajanikeetha12@gmail.com</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>tfv112</t>
-  </si>
-  <si>
-    <t>sai</t>
-  </si>
-  <si>
-    <t>skrisha12@thefirstventure.com</t>
-  </si>
-  <si>
-    <t>Team lead</t>
-  </si>
-  <si>
-    <t>TaxDep</t>
-  </si>
-  <si>
-    <t>tfv5</t>
-  </si>
-  <si>
-    <t>tfv114</t>
-  </si>
-  <si>
-    <t>Suneel</t>
-  </si>
-  <si>
-    <t>test12@gmail.com</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>tfv1</t>
-  </si>
-  <si>
-    <t>tfv113</t>
-  </si>
-  <si>
-    <t>Santosh</t>
-  </si>
-  <si>
-    <t>l.prasu1912@gmail.com</t>
-  </si>
-  <si>
-    <t>tfv2</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Empid Missing</t>
   </si>
 </sst>
 </file>
@@ -496,7 +400,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,181 +441,6 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>555</v>
-      </c>
-      <c r="G2">
-        <v>123456789</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>555</v>
-      </c>
-      <c r="G3">
-        <v>123456789</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>555</v>
-      </c>
-      <c r="G4">
-        <v>123456789</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5">
-        <v>555</v>
-      </c>
-      <c r="G5">
-        <v>123456789</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>1234567898</v>
-      </c>
-      <c r="G6">
-        <v>1258900</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -735,7 +464,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,76 +505,6 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changees for employee list
</commit_message>
<xml_diff>
--- a/wp-admin/error.xlsx
+++ b/wp-admin/error.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Employee Code</t>
   </si>
@@ -50,130 +50,22 @@
     <t>Error Message</t>
   </si>
   <si>
+    <t>tfv8</t>
+  </si>
+  <si>
+    <t>Emp123</t>
+  </si>
+  <si>
+    <t>tfv123@gmail.com</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
     <t>tfv1</t>
   </si>
   <si>
-    <t>Emp143</t>
-  </si>
-  <si>
-    <t>saiorkrish@gmail.com</t>
-  </si>
-  <si>
-    <t>Accounts</t>
-  </si>
-  <si>
-    <t>tfv3</t>
-  </si>
-  <si>
-    <t>Devloper</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Employee Email already Exists</t>
-  </si>
-  <si>
-    <t>tfv2</t>
-  </si>
-  <si>
-    <t>Emp144</t>
-  </si>
-  <si>
-    <t>test144@gmail.com</t>
-  </si>
-  <si>
-    <t>finance</t>
-  </si>
-  <si>
-    <t>tfv4</t>
-  </si>
-  <si>
     <t>---</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Emp145</t>
-  </si>
-  <si>
-    <t>test145@gmail.com</t>
-  </si>
-  <si>
-    <t>hr</t>
-  </si>
-  <si>
-    <t>tfv5</t>
-  </si>
-  <si>
-    <t>Programmer</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Emp146</t>
-  </si>
-  <si>
-    <t>test146@gmail.com</t>
-  </si>
-  <si>
-    <t>employee</t>
-  </si>
-  <si>
-    <t>tfv6</t>
-  </si>
-  <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>Emp147</t>
-  </si>
-  <si>
-    <t>saikrishna.b@corptne.com</t>
-  </si>
-  <si>
-    <t>approver</t>
-  </si>
-  <si>
-    <t>tfv7</t>
-  </si>
-  <si>
-    <t>Non-technical</t>
-  </si>
-  <si>
-    <t>tfv8</t>
-  </si>
-  <si>
-    <t>Emp148</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Emp149</t>
-  </si>
-  <si>
-    <t>test149@gmail.com</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Emp123</t>
-  </si>
-  <si>
-    <t>tfv123@gmail.com</t>
-  </si>
-  <si>
-    <t>manager</t>
   </si>
   <si>
     <t>Employee Grade Missing</t>
@@ -573,354 +465,109 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>56893025</v>
-      </c>
-      <c r="G2">
-        <v>123456</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3">
-        <v>123456</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>123456</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>123456</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6">
-        <v>123456</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <v>123456</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8">
-        <v>123456</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed row width issue
</commit_message>
<xml_diff>
--- a/wp-admin/error.xlsx
+++ b/wp-admin/error.xlsx
@@ -429,6 +429,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="34.134521" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
@@ -465,38 +473,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>